<commit_message>
Added all files from Dropbox/source_codes/competitions
</commit_message>
<xml_diff>
--- a/google-code-jam/Google Code Jam Statistic.xlsx
+++ b/google-code-jam/Google Code Jam Statistic.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="3435"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>YEAR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,23 +76,29 @@
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A,B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -126,6 +132,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -204,6 +215,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -238,6 +250,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,17 +426,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -532,6 +545,20 @@
       </c>
       <c r="C9" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -542,12 +569,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -555,12 +582,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>